<commit_message>
Added contacts table fucntionality
</commit_message>
<xml_diff>
--- a/Table Definitions/Tables.xlsx
+++ b/Table Definitions/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Code\Ditto\Table Definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDFA2F2-0420-4489-94C8-99CE83101CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2A6080-FBF8-44BF-97A7-694E146263C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6293C1F5-C8C1-4849-BDF2-D7A164F09DAD}"/>
   </bookViews>
@@ -429,12 +429,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -467,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -478,17 +484,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,112 +823,114 @@
   <dimension ref="B1:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="1.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="1.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="7" customWidth="1"/>
     <col min="9" max="9" width="1.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" customWidth="1"/>
     <col min="13" max="13" width="1.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="39.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="6.5703125" style="1" customWidth="1"/>
-    <col min="17" max="24" width="13.28515625" style="1" customWidth="1"/>
+    <col min="17" max="21" width="13.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" style="7" customWidth="1"/>
+    <col min="23" max="24" width="13.28515625" style="1" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>26</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="4"/>
+      <c r="R1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="6" t="s">
+      <c r="M3" s="5"/>
+      <c r="N3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="9" t="s">
         <v>114</v>
       </c>
       <c r="L4" t="s">
@@ -923,19 +941,19 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="9" t="s">
         <v>115</v>
       </c>
       <c r="L5"/>
@@ -944,19 +962,19 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="9" t="s">
         <v>116</v>
       </c>
       <c r="L6"/>
@@ -965,19 +983,19 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="9" t="s">
         <v>117</v>
       </c>
       <c r="L7"/>
@@ -986,19 +1004,19 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="9" t="s">
         <v>118</v>
       </c>
       <c r="L8"/>
@@ -1007,19 +1025,19 @@
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="9" t="s">
         <v>119</v>
       </c>
       <c r="L9"/>
@@ -1028,73 +1046,73 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J10"/>
+      <c r="J10" s="9"/>
       <c r="L10"/>
       <c r="N10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J11"/>
+      <c r="J11" s="9"/>
       <c r="L11"/>
       <c r="N11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="J12"/>
+      <c r="J12" s="9"/>
       <c r="L12"/>
       <c r="N12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="9" t="s">
         <v>87</v>
       </c>
       <c r="N13" t="s">
@@ -1102,13 +1120,13 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="7" t="s">
         <v>71</v>
       </c>
       <c r="N14" t="s">
@@ -1116,13 +1134,13 @@
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="7" t="s">
         <v>72</v>
       </c>
       <c r="N15" t="s">
@@ -1130,13 +1148,13 @@
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="7" t="s">
         <v>73</v>
       </c>
       <c r="N16" t="s">
@@ -1144,10 +1162,10 @@
       </c>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
+      <c r="F17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="7" t="s">
         <v>74</v>
       </c>
       <c r="N17" t="s">
@@ -1155,10 +1173,10 @@
       </c>
     </row>
     <row r="18" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+      <c r="F18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="7" t="s">
         <v>111</v>
       </c>
       <c r="N18" t="s">
@@ -1166,10 +1184,10 @@
       </c>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+      <c r="F19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="7" t="s">
         <v>112</v>
       </c>
       <c r="N19" t="s">
@@ -1177,7 +1195,7 @@
       </c>
     </row>
     <row r="20" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
+      <c r="F20" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N20" t="s">
@@ -1185,7 +1203,7 @@
       </c>
     </row>
     <row r="21" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
+      <c r="F21" s="9" t="s">
         <v>51</v>
       </c>
       <c r="N21" t="s">
@@ -1193,7 +1211,7 @@
       </c>
     </row>
     <row r="22" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+      <c r="F22" s="9" t="s">
         <v>52</v>
       </c>
       <c r="N22" t="s">
@@ -1201,7 +1219,7 @@
       </c>
     </row>
     <row r="23" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+      <c r="F23" s="9" t="s">
         <v>53</v>
       </c>
       <c r="N23" t="s">
@@ -1209,7 +1227,7 @@
       </c>
     </row>
     <row r="24" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
+      <c r="F24" s="9" t="s">
         <v>54</v>
       </c>
       <c r="N24" t="s">
@@ -1217,7 +1235,7 @@
       </c>
     </row>
     <row r="25" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
+      <c r="F25" s="9" t="s">
         <v>55</v>
       </c>
       <c r="N25" t="s">
@@ -1225,7 +1243,7 @@
       </c>
     </row>
     <row r="26" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
+      <c r="F26" s="9" t="s">
         <v>56</v>
       </c>
       <c r="N26" t="s">
@@ -1233,7 +1251,7 @@
       </c>
     </row>
     <row r="27" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
+      <c r="F27" s="9" t="s">
         <v>57</v>
       </c>
       <c r="N27" t="s">
@@ -1241,7 +1259,7 @@
       </c>
     </row>
     <row r="28" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+      <c r="F28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="N28" t="s">
@@ -1249,7 +1267,7 @@
       </c>
     </row>
     <row r="29" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+      <c r="F29" s="9" t="s">
         <v>17</v>
       </c>
       <c r="N29" t="s">
@@ -1257,7 +1275,7 @@
       </c>
     </row>
     <row r="30" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+      <c r="F30" s="9" t="s">
         <v>59</v>
       </c>
       <c r="N30" t="s">
@@ -1265,7 +1283,7 @@
       </c>
     </row>
     <row r="31" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
+      <c r="F31" s="9" t="s">
         <v>60</v>
       </c>
       <c r="N31" t="s">
@@ -1273,7 +1291,7 @@
       </c>
     </row>
     <row r="32" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+      <c r="F32" s="9" t="s">
         <v>61</v>
       </c>
       <c r="N32" t="s">
@@ -1281,7 +1299,7 @@
       </c>
     </row>
     <row r="33" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
+      <c r="F33" s="9" t="s">
         <v>16</v>
       </c>
       <c r="N33" t="s">
@@ -1289,7 +1307,7 @@
       </c>
     </row>
     <row r="34" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
+      <c r="F34" s="9" t="s">
         <v>62</v>
       </c>
       <c r="N34" t="s">
@@ -1297,7 +1315,7 @@
       </c>
     </row>
     <row r="35" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="11" t="s">
         <v>69</v>
       </c>
       <c r="N35" t="s">
@@ -1305,7 +1323,7 @@
       </c>
     </row>
     <row r="36" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="11" t="s">
         <v>70</v>
       </c>
       <c r="N36" t="s">
@@ -1313,7 +1331,7 @@
       </c>
     </row>
     <row r="37" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="11" t="s">
         <v>110</v>
       </c>
       <c r="N37" t="s">
@@ -1321,7 +1339,7 @@
       </c>
     </row>
     <row r="38" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="11" t="s">
         <v>113</v>
       </c>
       <c r="N38" t="s">

</xml_diff>